<commit_message>
Updated the Code for APIs
</commit_message>
<xml_diff>
--- a/TestData/API_INPUT.xlsx
+++ b/TestData/API_INPUT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaik.hussain\git\HDAP2_PEGAUI_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\HDAP2_PEGAUI_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D27756-9522-463E-81D1-62B926E0D68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330FC65C-99D6-4ACF-8107-1E9BB3E372B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{11F28E78-D351-4DCD-933B-0501C50198D8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{11F28E78-D351-4DCD-933B-0501C50198D8}"/>
   </bookViews>
   <sheets>
     <sheet name="ChaseData" sheetId="2" r:id="rId1"/>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -41,13 +30,13 @@
     <t>RGID</t>
   </si>
   <si>
-    <t>RG-34565541998716</t>
+    <t>Prvoider</t>
   </si>
   <si>
-    <t>F-147747020225</t>
+    <t>RG-20002</t>
   </si>
   <si>
-    <t>Prvoider</t>
+    <t>P-388412033222</t>
   </si>
 </sst>
 </file>
@@ -453,7 +442,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,15 +456,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code for RG
</commit_message>
<xml_diff>
--- a/TestData/API_INPUT.xlsx
+++ b/TestData/API_INPUT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\HDAP2_PEGAUI_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaik.hussain\git\HDAP2_PEGAUI_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330FC65C-99D6-4ACF-8107-1E9BB3E372B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8510081-47AB-4384-9A43-A2957DAE954E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{11F28E78-D351-4DCD-933B-0501C50198D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{11F28E78-D351-4DCD-933B-0501C50198D8}"/>
   </bookViews>
   <sheets>
     <sheet name="ChaseData" sheetId="2" r:id="rId1"/>
@@ -33,10 +33,10 @@
     <t>Prvoider</t>
   </si>
   <si>
-    <t>RG-20002</t>
+    <t>RG-34565541998716</t>
   </si>
   <si>
-    <t>P-388412033222</t>
+    <t>P-535468020225</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Completed the code for Facility and Practitioner Get API
</commit_message>
<xml_diff>
--- a/TestData/API_INPUT.xlsx
+++ b/TestData/API_INPUT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaik.hussain\git\HDAP2_PEGAUI_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\HDAP2_PEGAUI_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8510081-47AB-4384-9A43-A2957DAE954E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5871B95-D137-4A93-919C-0D3C4EC43F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{11F28E78-D351-4DCD-933B-0501C50198D8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{11F28E78-D351-4DCD-933B-0501C50198D8}"/>
   </bookViews>
   <sheets>
     <sheet name="ChaseData" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <t>RG-34565541998716</t>
   </si>
   <si>
-    <t>P-535468020225</t>
+    <t>F-147747020225</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update the code for Practitioner
Get API for the Practitioner is completed
</commit_message>
<xml_diff>
--- a/TestData/API_INPUT.xlsx
+++ b/TestData/API_INPUT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\HDAP2_PEGAUI_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaik.hussain\git\HDAP2_PEGAUI_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5871B95-D137-4A93-919C-0D3C4EC43F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93919B1-F5CA-42A1-8D5B-F894457E4EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{11F28E78-D351-4DCD-933B-0501C50198D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{11F28E78-D351-4DCD-933B-0501C50198D8}"/>
   </bookViews>
   <sheets>
     <sheet name="ChaseData" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>RGID</t>
   </si>
@@ -33,10 +33,13 @@
     <t>Prvoider</t>
   </si>
   <si>
-    <t>RG-34565541998716</t>
+    <t>RG-20002</t>
   </si>
   <si>
-    <t>F-147747020225</t>
+    <t>P-388412033222</t>
+  </si>
+  <si>
+    <t>F-468464031024</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,16 +442,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B518E2B7-85F6-47DD-AC50-F01E66D54E34}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -467,7 +470,16 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the code to read from Excel Sheet
Updated the code to read from Excel Sheet
</commit_message>
<xml_diff>
--- a/TestData/API_INPUT.xlsx
+++ b/TestData/API_INPUT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaik.hussain\git\HDAP2_PEGAUI_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\git\HDAP2_PEGAUI_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53F3049-166D-4FEC-880D-E8269B274F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA7872A-F854-47D2-9F52-A666B6D52867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{11F28E78-D351-4DCD-933B-0501C50198D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{11F28E78-D351-4DCD-933B-0501C50198D8}"/>
   </bookViews>
   <sheets>
     <sheet name="ChaseData" sheetId="2" r:id="rId1"/>
@@ -25,18 +25,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>RGID</t>
   </si>
   <si>
-    <t>Prvoider</t>
-  </si>
-  <si>
-    <t>RG-20002</t>
-  </si>
-  <si>
-    <t>P-388412033222</t>
+    <t>Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run </t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>ProviderID</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>RG-35022</t>
+  </si>
+  <si>
+    <t>P-157855884725</t>
+  </si>
+  <si>
+    <t>testcase</t>
+  </si>
+  <si>
+    <t>"3"</t>
   </si>
 </sst>
 </file>
@@ -101,10 +122,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,40 +465,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B518E2B7-85F6-47DD-AC50-F01E66D54E34}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read From Excel Sheet
</commit_message>
<xml_diff>
--- a/TestData/API_INPUT.xlsx
+++ b/TestData/API_INPUT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\git\HDAP2_PEGAUI_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaik.hussain\git\HDAP2_PEGAUI_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA7872A-F854-47D2-9F52-A666B6D52867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF0E18F-CDF3-41A4-ABC4-FF442CCC1E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{11F28E78-D351-4DCD-933B-0501C50198D8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>RGID</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>"3"</t>
+  </si>
+  <si>
+    <t>AccountID</t>
+  </si>
+  <si>
+    <t>SubAccountID</t>
+  </si>
+  <si>
+    <t>P610</t>
+  </si>
+  <si>
+    <t>Z888</t>
   </si>
 </sst>
 </file>
@@ -95,7 +107,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -118,11 +130,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -131,6 +156,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B518E2B7-85F6-47DD-AC50-F01E66D54E34}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,11 +503,12 @@
     <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -499,11 +527,17 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -518,6 +552,12 @@
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with Random First Name and Last Name
</commit_message>
<xml_diff>
--- a/TestData/API_INPUT.xlsx
+++ b/TestData/API_INPUT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaik.hussain\git\HDAP2_PEGAUI_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\git\HDAP2_PEGAUI_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1A7C1C-8D65-41E6-8DE9-458F86FDAF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF825926-796F-4937-A6B7-02FD167449F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{11F28E78-D351-4DCD-933B-0501C50198D8}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="42">
   <si>
     <t>RGID</t>
   </si>
@@ -65,30 +63,12 @@
     <t>SubAccountID</t>
   </si>
   <si>
-    <t>RG-36024</t>
-  </si>
-  <si>
-    <t>P-196212245725</t>
-  </si>
-  <si>
     <t>"5"</t>
   </si>
   <si>
     <t>M900</t>
   </si>
   <si>
-    <t>S418</t>
-  </si>
-  <si>
-    <t>set1</t>
-  </si>
-  <si>
-    <t>set2</t>
-  </si>
-  <si>
-    <t>set3</t>
-  </si>
-  <si>
     <t>RG-36010</t>
   </si>
   <si>
@@ -98,48 +78,15 @@
     <t>P-157855884725</t>
   </si>
   <si>
-    <t>P610</t>
-  </si>
-  <si>
-    <t>Z888</t>
-  </si>
-  <si>
-    <t>set5</t>
-  </si>
-  <si>
     <t>P-134669792725</t>
   </si>
   <si>
-    <t>"3"</t>
-  </si>
-  <si>
     <t>"2"</t>
   </si>
   <si>
-    <t>set6</t>
-  </si>
-  <si>
-    <t>set7</t>
-  </si>
-  <si>
-    <t>P700</t>
-  </si>
-  <si>
-    <t>set8</t>
-  </si>
-  <si>
-    <t>S154</t>
-  </si>
-  <si>
     <t>"10"</t>
   </si>
   <si>
-    <t>RG-38003</t>
-  </si>
-  <si>
-    <t>P-7040916072</t>
-  </si>
-  <si>
     <t>P-183111916325</t>
   </si>
   <si>
@@ -149,24 +96,6 @@
     <t>UAT</t>
   </si>
   <si>
-    <t>set9</t>
-  </si>
-  <si>
-    <t>FS01</t>
-  </si>
-  <si>
-    <t>H090</t>
-  </si>
-  <si>
-    <t>RG-11006</t>
-  </si>
-  <si>
-    <t>P-388412088777</t>
-  </si>
-  <si>
-    <t>set10</t>
-  </si>
-  <si>
     <t>Z610</t>
   </si>
   <si>
@@ -182,18 +111,6 @@
     <t>F-406112020824</t>
   </si>
   <si>
-    <t>set11</t>
-  </si>
-  <si>
-    <t>set444</t>
-  </si>
-  <si>
-    <t>set4444</t>
-  </si>
-  <si>
-    <t>set12</t>
-  </si>
-  <si>
     <t>DEV</t>
   </si>
   <si>
@@ -206,34 +123,43 @@
     <t>RG-44004</t>
   </si>
   <si>
-    <t>set13</t>
-  </si>
-  <si>
     <t>P-185162478725</t>
   </si>
   <si>
     <t>G444</t>
   </si>
   <si>
-    <t>Demo1</t>
-  </si>
-  <si>
     <t>O900</t>
   </si>
   <si>
     <t>Q888</t>
   </si>
   <si>
-    <t>Demo12</t>
-  </si>
-  <si>
-    <t>UAT1</t>
-  </si>
-  <si>
-    <t>UAT21</t>
-  </si>
-  <si>
     <t>P888</t>
+  </si>
+  <si>
+    <t>QASet1</t>
+  </si>
+  <si>
+    <t>UATSet1</t>
+  </si>
+  <si>
+    <t>QASet2</t>
+  </si>
+  <si>
+    <t>QASet3</t>
+  </si>
+  <si>
+    <t>QASet4</t>
+  </si>
+  <si>
+    <t>QASet5</t>
+  </si>
+  <si>
+    <t>QASet6</t>
+  </si>
+  <si>
+    <t>QASet7</t>
   </si>
 </sst>
 </file>
@@ -271,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -294,37 +220,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -334,8 +234,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B518E2B7-85F6-47DD-AC50-F01E66D54E34}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,7 +587,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -712,19 +610,19 @@
       <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>14</v>
+      <c r="I1" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
@@ -733,15 +631,15 @@
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -765,18 +663,18 @@
         <v>8</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>3</v>
@@ -785,15 +683,15 @@
         <v>6</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
@@ -816,19 +714,19 @@
       <c r="H5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>15</v>
+      <c r="I5" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>3</v>
@@ -837,15 +735,15 @@
         <v>6</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
@@ -868,19 +766,19 @@
       <c r="H7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>16</v>
+      <c r="I7" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>3</v>
@@ -889,15 +787,15 @@
         <v>6</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>0</v>
@@ -920,36 +818,36 @@
       <c r="H9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>63</v>
+      <c r="I9" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>34</v>
+      <c r="B10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>0</v>
@@ -972,19 +870,19 @@
       <c r="H11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>50</v>
+      <c r="I11" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>3</v>
@@ -993,15 +891,15 @@
         <v>6</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>0</v>
@@ -1024,19 +922,19 @@
       <c r="H13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>22</v>
+      <c r="I13" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>3</v>
@@ -1045,15 +943,15 @@
         <v>6</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>0</v>
@@ -1076,499 +974,31 @@
       <c r="H15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>26</v>
+      <c r="I15" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>